<commit_message>
Data normalization excel file.
</commit_message>
<xml_diff>
--- a/documentation/DataNormalization.xlsx
+++ b/documentation/DataNormalization.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="411" documentId="11_F25DC773A252ABDACC104811A15A7A1C5BDE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4810A724-785F-4D59-8110-993042A4C027}"/>
   <bookViews>
-    <workbookView xWindow="20380" yWindow="-6870" windowWidth="21600" windowHeight="12530" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Normalization" sheetId="1" r:id="rId1"/>
@@ -848,9 +848,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{340D9615-31C4-4DF1-9E1C-C3891E283E6D}">
   <dimension ref="A1:AW5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AE1" workbookViewId="0">
-      <selection activeCell="AX3" sqref="AX3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>